<commit_message>
CO2RR MSP: poor performance
</commit_message>
<xml_diff>
--- a/github/workflows/Hyein/multkan_sweep_autosave/CO2RR_MSP_20251106_0906.xlsx
+++ b/github/workflows/Hyein/multkan_sweep_autosave/CO2RR_MSP_20251106_0906.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pykan\github\workflows\Hyein\multkan_sweep_autosave\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{496664BF-73CE-45EF-89E4-EE1E5D81D8A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0916C343-BAB6-4D33-98F0-0D98B84C09F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2510" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2512" uniqueCount="109">
   <si>
     <t>r2_train</t>
   </si>
@@ -388,6 +388,14 @@
   <si>
     <t>spline_test_loss_std</t>
   </si>
+  <si>
+    <t>Success</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>lamb</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -451,9 +459,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -31856,7 +31867,7 @@
   <dimension ref="A1:AB501"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AB6" sqref="AB6"/>
+      <selection activeCell="AD14" sqref="AD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -31934,6 +31945,12 @@
       <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="AA1" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2">

</xml_diff>